<commit_message>
updated excel spreadsheet of flows in each channel based on latest orificing calc
</commit_message>
<xml_diff>
--- a/BnB/channelFlows.xlsx
+++ b/BnB/channelFlows.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-51120" yWindow="440" windowWidth="25560" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="-38320" yWindow="440" windowWidth="19160" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>chan1</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>W0 (kg/s/pin)</t>
+  </si>
+  <si>
+    <t>chan5</t>
+  </si>
+  <si>
+    <t>chan7</t>
   </si>
 </sst>
 </file>
@@ -362,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G256"/>
+  <dimension ref="A1:J256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -373,7 +379,7 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -387,2065 +393,2090 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
         <f>AVERAGE(B5:B46)</f>
-        <v>23.719395428571435</v>
+        <v>26.806676829268284</v>
       </c>
       <c r="C2">
         <f>AVERAGE(C5:C88)</f>
-        <v>89.363536666666647</v>
+        <v>86.526643433734776</v>
       </c>
       <c r="D2">
         <f>AVERAGE(D5:D130)</f>
-        <v>70.611205571428613</v>
+        <v>68.650238952380988</v>
       </c>
       <c r="E2">
         <f>AVERAGE(E5:E256)</f>
-        <v>4.3297779166666341</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5.7326002619047696</v>
+      </c>
+      <c r="G2" t="e">
+        <f>AVERAGE(G5:G220)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I2">
+        <f>I5</f>
+        <v>17.313586000000001</v>
+      </c>
+      <c r="J2">
+        <v>89.309960000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <f>B2/169</f>
-        <v>0.14035145224006765</v>
+        <v>0.15861938952229754</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:E3" si="0">C2/169</f>
-        <v>0.5287783234714003</v>
+        <v>0.51199197298067911</v>
       </c>
       <c r="D3">
         <f t="shared" si="0"/>
-        <v>0.41781778444632317</v>
+        <v>0.40621443167089344</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>2.5619987672583635E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3.3920711608903961E-2</v>
+      </c>
+      <c r="I3">
+        <f>I2/169</f>
+        <v>0.10244725443786983</v>
+      </c>
+      <c r="J3">
+        <f>J2/169</f>
+        <v>0.52846130177514794</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
       <c r="C5">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D5">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E5">
-        <v>4.3378740000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5.7224110000000001</v>
+      </c>
+      <c r="I5">
+        <v>17.313586000000001</v>
+      </c>
+      <c r="J5">
+        <v>89.309960000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
       <c r="C6">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D6">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E6">
-        <v>12.658714</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17.313586000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
       <c r="C7">
-        <v>72.021572000000006</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D7">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E7">
-        <v>15.615853</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21.943339000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
       <c r="C8">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D8">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E8">
-        <v>12.658714</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11.630065</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
       <c r="C9">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D9">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E9">
-        <v>18.936429</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27.553781000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>12.658714</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C10">
-        <v>72.021572000000006</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D10">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E10">
-        <v>18.936429</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27.553781000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>18.936429</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C11">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D11">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E11">
-        <v>18.936429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>27.553781000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C12">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D12">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E12">
-        <v>12.658714</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11.630065</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13">
-        <v>18.936429</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C13">
-        <v>72.021572000000006</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D13">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E13">
-        <v>15.615853</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>21.943339000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C14">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D14">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E14">
-        <v>12.658714</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17.313586000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15">
-        <v>18.936429</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C15">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D15">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E15">
-        <v>4.3378740000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>5.7224110000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C16">
-        <v>72.021572000000006</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D16">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E16">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17">
-        <v>18.936429</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C17">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D17">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E17">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C18">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D18">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E18">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19">
-        <v>18.936429</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C19">
-        <v>72.021572000000006</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D19">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E19">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C20">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D20">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E20">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21">
-        <v>18.936429</v>
+        <v>21.943339000000002</v>
       </c>
       <c r="C21">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D21">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E21">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>15.615853</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="C22">
-        <v>72.021572000000006</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D22">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E22">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C23">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D23">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E23">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C24">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D24">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E24">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25">
-        <v>27.444873000000001</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="C25">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D25">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E25">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C26">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D26">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E26">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C27">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D27">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E27">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28">
-        <v>27.444873000000001</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="C28">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D28">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E28">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C29">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D29">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E29">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C30">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D30">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E30">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B31">
-        <v>27.444873000000001</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="C31">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D31">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E31">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C32">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D32">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E32">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C33">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D33">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E33">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34">
-        <v>27.444873000000001</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="C34">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D34">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E34">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C35">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D35">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E35">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B36">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C36">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D36">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E36">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37">
-        <v>27.444873000000001</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="C37">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D37">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E37">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B38">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C38">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D38">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E38">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39">
-        <v>27.444873000000001</v>
+        <v>27.553781000000001</v>
       </c>
       <c r="C39">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D39">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E39">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B40">
-        <v>27.444873000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="C40">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D40">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E40">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="C41">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D41">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E41">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="C42">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D42">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E42">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="C43">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D43">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E43">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="C44">
-        <v>95.654216000000005</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D44">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E44">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="C45">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="D45">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E45">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B46">
-        <v>36.490152999999999</v>
-      </c>
       <c r="C46">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D46">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E46">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C47">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D47">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E47">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C48">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D48">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E48">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C49">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D49">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E49">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C50">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D50">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E50">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C51">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D51">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E51">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C52">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D52">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E52">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C53">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D53">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E53">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C54">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D54">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E54">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C55">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D55">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E55">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C56">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D56">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E56">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C57">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D57">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E57">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C58">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D58">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E58">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C59">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D59">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E59">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C60">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D60">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E60">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C61">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D61">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E61">
-        <v>18.936429</v>
+        <v>27.553781000000001</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C62">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D62">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E62">
-        <v>12.658714</v>
+        <v>11.630065</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C63">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D63">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E63">
-        <v>15.615853</v>
+        <v>21.943339000000002</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C64">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D64">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E64">
-        <v>12.658714</v>
+        <v>17.313586000000001</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C65">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D65">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E65">
-        <v>0.91756499999999996</v>
+        <v>1.2342409999999999</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C66">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D66">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E66">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C67">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D67">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E67">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C68">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D68">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E68">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C69">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D69">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E69">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C70">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D70">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E70">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C71">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D71">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E71">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C72">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D72">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E72">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C73">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D73">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E73">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C74">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D74">
-        <v>81.846316000000002</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="E74">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="75" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C75">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D75">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E75">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="76" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C76">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D76">
-        <v>81.846316000000002</v>
+        <v>80.069349000000003</v>
       </c>
       <c r="E76">
-        <v>0.91756499999999996</v>
+        <v>1.2342409999999999</v>
       </c>
     </row>
     <row r="77" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C77">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D77">
-        <v>81.846316000000002</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="E77">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="78" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C78">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D78">
-        <v>81.846316000000002</v>
+        <v>38.098796</v>
       </c>
       <c r="E78">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="79" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C79">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D79">
-        <v>81.846316000000002</v>
+        <v>38.098796</v>
       </c>
       <c r="E79">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="80" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C80">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D80">
-        <v>81.846316000000002</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E80">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C81">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D81">
-        <v>81.846316000000002</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E81">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C82">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D82">
-        <v>81.846316000000002</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E82">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C83">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D83">
-        <v>81.846316000000002</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E83">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C84">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D84">
-        <v>81.846316000000002</v>
+        <v>38.098796</v>
       </c>
       <c r="E84">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C85">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D85">
-        <v>81.846316000000002</v>
+        <v>38.098796</v>
       </c>
       <c r="E85">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C86">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D86">
-        <v>81.846316000000002</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="E86">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="87" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C87">
-        <v>95.654216000000005</v>
+        <v>89.309960000000004</v>
       </c>
       <c r="D87">
-        <v>81.846316000000002</v>
+        <v>38.098796</v>
       </c>
       <c r="E87">
-        <v>0.91756499999999996</v>
+        <v>1.2342409999999999</v>
       </c>
     </row>
     <row r="88" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C88">
-        <v>95.654216000000005</v>
-      </c>
       <c r="D88">
-        <v>81.846316000000002</v>
+        <v>38.098796</v>
       </c>
       <c r="E88">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D89">
-        <v>27.444873000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E89">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="90" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D90">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E90">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D91">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E91">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="92" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D92">
-        <v>40.367004000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E92">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="93" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D93">
-        <v>40.367004000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E93">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="94" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D94">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E94">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D95">
-        <v>36.490152999999999</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="E95">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="96" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D96">
-        <v>27.444873000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E96">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="97" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D97">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E97">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="98" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D98">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E98">
-        <v>0.91756499999999996</v>
+        <v>1.2342409999999999</v>
       </c>
     </row>
     <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99">
-        <v>40.367004000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E99">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100">
-        <v>40.367004000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E100">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E101">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E102">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103">
-        <v>27.444873000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E103">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104">
-        <v>36.490152999999999</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="E104">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E105">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106">
-        <v>40.367004000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E106">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107">
-        <v>40.367004000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E107">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E108">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E109">
-        <v>0.91756499999999996</v>
+        <v>1.2342409999999999</v>
       </c>
     </row>
     <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110">
-        <v>27.444873000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E110">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E111">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="112" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D112">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E112">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="113" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D113">
-        <v>40.367004000000001</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="E113">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="114" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D114">
-        <v>40.367004000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E114">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="115" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D115">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E115">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="116" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D116">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E116">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="117" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D117">
-        <v>27.444873000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E117">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="118" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D118">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E118">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="119" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D119">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E119">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="120" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D120">
-        <v>40.367004000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E120">
-        <v>0.91756499999999996</v>
+        <v>1.2342409999999999</v>
       </c>
     </row>
     <row r="121" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D121">
-        <v>40.367004000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E121">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="122" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D122">
-        <v>36.490152999999999</v>
+        <v>31.657934000000001</v>
       </c>
       <c r="E122">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="123" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D123">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E123">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="124" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D124">
-        <v>27.444873000000001</v>
+        <v>38.098796</v>
       </c>
       <c r="E124">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="125" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D125">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E125">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="126" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D126">
-        <v>36.490152999999999</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E126">
-        <v>4.3378740000000002</v>
+        <v>5.7224110000000001</v>
       </c>
     </row>
     <row r="127" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D127">
-        <v>40.367004000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E127">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="128" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D128">
-        <v>40.367004000000001</v>
+        <v>55.711205999999997</v>
       </c>
       <c r="E128">
-        <v>2.666185</v>
+        <v>3.4040780000000002</v>
       </c>
     </row>
     <row r="129" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D129">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E129">
-        <v>3.0479270000000001</v>
+        <v>3.9397929999999999</v>
       </c>
     </row>
     <row r="130" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D130">
-        <v>36.490152999999999</v>
+        <v>38.098796</v>
       </c>
       <c r="E130">
-        <v>1.6267750000000001</v>
+        <v>2.1684290000000002</v>
       </c>
     </row>
     <row r="131" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E131">
-        <v>0.230852</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="132" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E132">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="133" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E133">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="134" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E134">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="135" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E135">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="136" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E136">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="137" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E137">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="138" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E138">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="139" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E139">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="140" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E140">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="141" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E141">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="142" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E142">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="143" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E143">
-        <v>0.230852</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="144" spans="4:5" x14ac:dyDescent="0.2">
       <c r="E144">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E145">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="146" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E146">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="147" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E147">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="148" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E148">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="149" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E149">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="150" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E150">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="151" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E151">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="152" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E152">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="153" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E153">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="154" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E154">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="155" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E155">
-        <v>0.230852</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="156" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E156">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="157" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E157">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="158" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E158">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="159" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E159">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="160" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E160">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="161" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E161">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="162" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E162">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="163" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E163">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="164" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E164">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="165" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E165">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="166" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E166">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="167" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E167">
-        <v>0.230852</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="168" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E168">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="169" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E169">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="170" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E170">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="171" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E171">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="172" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E172">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="173" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E173">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="174" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E174">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="175" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E175">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="176" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E176">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="177" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E177">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="178" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E178">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="179" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E179">
-        <v>0.230852</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="180" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E180">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="181" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E181">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="182" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E182">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="183" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E183">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="184" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E184">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="185" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E185">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="186" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E186">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="187" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E187">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="188" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E188">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="189" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E189">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="190" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E190">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="191" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E191">
-        <v>0.230852</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="192" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E192">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="193" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E193">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="194" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E194">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="195" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E195">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="196" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E196">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="197" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E197">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="198" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E198">
-        <v>0.71513300000000002</v>
+        <v>1.069866</v>
       </c>
     </row>
     <row r="199" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E199">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="200" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E200">
-        <v>0.71513300000000002</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="201" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E201">
-        <v>0.54137199999999996</v>
+        <v>0.77271299999999998</v>
       </c>
     </row>
     <row r="202" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E202">
-        <v>0.30868299999999999</v>
+        <v>0.40931000000000001</v>
       </c>
     </row>
     <row r="203" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E203">
-        <v>0.17961199999999999</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="204" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E204">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="205" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E205">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="206" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E206">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="207" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E207">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="208" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E208">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="209" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E209">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="210" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E210">
-        <v>0.12811600000000001</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="211" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E211">
-        <v>0.12811600000000001</v>
+        <v>0.14152899999999999</v>
       </c>
     </row>
     <row r="212" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E212">
-        <v>0.17961199999999999</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="213" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E213">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="214" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E214">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="215" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E215">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="216" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E216">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="217" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E217">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="218" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E218">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="219" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E219">
-        <v>0.12811600000000001</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="220" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E220">
-        <v>0.12811600000000001</v>
+        <v>0.14152899999999999</v>
       </c>
     </row>
     <row r="221" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E221">
-        <v>0.17961199999999999</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="222" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E222">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="223" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E223">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="224" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E224">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="225" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E225">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="226" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E226">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="227" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E227">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="228" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E228">
-        <v>0.12811600000000001</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="229" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E229">
-        <v>0.12811600000000001</v>
+        <v>0.14152899999999999</v>
       </c>
     </row>
     <row r="230" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E230">
-        <v>0.17961199999999999</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="231" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E231">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="232" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E232">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="233" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E233">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="234" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E234">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="235" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E235">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="236" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E236">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="237" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E237">
-        <v>0.12811600000000001</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="238" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E238">
-        <v>0.12811600000000001</v>
+        <v>0.14152899999999999</v>
       </c>
     </row>
     <row r="239" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E239">
-        <v>0.17961199999999999</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="240" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E240">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="241" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E241">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="242" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E242">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="243" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E243">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="244" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E244">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="245" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E245">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="246" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E246">
-        <v>0.12811600000000001</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="247" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E247">
-        <v>0.12811600000000001</v>
+        <v>0.14152899999999999</v>
       </c>
     </row>
     <row r="248" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E248">
-        <v>0.17961199999999999</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="249" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E249">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="250" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E250">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="251" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E251">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="252" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E252">
-        <v>0.230852</v>
+        <v>0.31857400000000002</v>
       </c>
     </row>
     <row r="253" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E253">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="254" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E254">
-        <v>0.17961199999999999</v>
+        <v>0.24097499999999999</v>
       </c>
     </row>
     <row r="255" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E255">
-        <v>0.12811600000000001</v>
+        <v>0.19009000000000001</v>
       </c>
     </row>
     <row r="256" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E256">
-        <v>0.12811600000000001</v>
+        <v>0.14152899999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>